<commit_message>
Se crea formato para conteo
</commit_message>
<xml_diff>
--- a/JoanneFigueroa/ModeloReporte.xlsx
+++ b/JoanneFigueroa/ModeloReporte.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Criptodev\Clientes\Mariano\JoanneFigueroa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos\Mariano\JoanneFigueroa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADC9A8A-A1F2-48E7-92BD-3C19E13CD196}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B8FC6F-D5AE-490D-B438-DF2A1510D9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{8B72A0A4-6553-C340-9843-EC5DA5351AC0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8B72A0A4-6553-C340-9843-EC5DA5351AC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
   <si>
     <t>I</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>+=daño profundo al tejido</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -556,6 +559,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,187 +581,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>665124</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>113386</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07912D06-1E5B-4735-966D-DABF7B63521C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="13009524" cy="7314286"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>665124</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>113386</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBB02BF8-784A-463F-A889-E2B62AC0B546}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="7600950"/>
-          <a:ext cx="13009524" cy="7314286"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>665124</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>113386</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E737C8B-95E6-4478-A2A4-27D87D460F2A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="15001875"/>
-          <a:ext cx="13009524" cy="7314286"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>112</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>665124</xdr:colOff>
-      <xdr:row>148</xdr:row>
-      <xdr:rowOff>113386</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17D57B97-C368-4616-B153-1450AC57F27A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="22402800"/>
-          <a:ext cx="13009524" cy="7314286"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1053,10 +881,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABB8180-567C-1241-B6E8-35630945327C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1072,7 +900,7 @@
     <col min="9" max="9" width="6.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="47" t="s">
         <v>56</v>
       </c>
@@ -1080,7 +908,7 @@
       <c r="C1" s="47"/>
       <c r="D1" s="47"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>58</v>
       </c>
@@ -1088,7 +916,7 @@
       <c r="C2" s="48"/>
       <c r="D2" s="48"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>57</v>
       </c>
@@ -1096,15 +924,15 @@
         <v>44446</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>34</v>
       </c>
@@ -1118,7 +946,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
@@ -1131,11 +959,13 @@
       <c r="F7" t="s">
         <v>67</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="52" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11" t="s">
@@ -1148,8 +978,11 @@
       <c r="F8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11" t="s">
@@ -1162,8 +995,11 @@
       <c r="F9" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
@@ -1176,8 +1012,11 @@
       <c r="F10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11" t="s">
@@ -1190,8 +1029,11 @@
       <c r="F11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16" t="s">
@@ -1204,16 +1046,19 @@
         <f>SUM(D7:D12)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>0</v>
       </c>
@@ -1224,7 +1069,7 @@
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="12" t="s">
         <v>1</v>
@@ -1311,15 +1156,23 @@
       <c r="F21" t="s">
         <v>66</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="52" t="s">
         <v>69</v>
       </c>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D22" s="2"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="2"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
     </row>
     <row r="24" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
@@ -1336,9 +1189,15 @@
       <c r="F24" t="s">
         <v>66</v>
       </c>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
     </row>
     <row r="25" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="3"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
@@ -1350,6 +1209,9 @@
       <c r="C26" s="25"/>
       <c r="D26" s="26"/>
       <c r="E26" s="25"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
@@ -1409,7 +1271,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="27" t="s">
@@ -1422,10 +1284,10 @@
       <c r="F31" t="s">
         <v>67</v>
       </c>
-      <c r="H31" t="e">
-        <f>daño profundo al tejido</f>
-        <v>#NAME?</v>
-      </c>
+      <c r="G31" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" s="53"/>
       <c r="I31" t="s">
         <v>66</v>
       </c>
@@ -1443,8 +1305,10 @@
       <c r="F32" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11" t="s">
         <v>14</v>
@@ -1457,8 +1321,10 @@
       <c r="F33" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11" t="s">
         <v>16</v>
@@ -1473,8 +1339,10 @@
       <c r="F34" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11" t="s">
@@ -1488,7 +1356,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11" t="s">
@@ -1502,7 +1370,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11" t="s">
         <v>64</v>
@@ -1516,7 +1384,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="11" t="s">
         <v>65</v>
@@ -1530,7 +1398,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11" t="s">
         <v>20</v>
@@ -1544,7 +1412,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11" t="s">
         <v>21</v>
@@ -1558,7 +1426,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="11" t="s">
         <v>22</v>
@@ -1572,7 +1440,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="11" t="s">
         <v>23</v>
@@ -1586,7 +1454,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="11" t="s">
         <v>24</v>
@@ -1600,7 +1468,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="11" t="s">
         <v>25</v>
@@ -1614,7 +1482,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="11" t="s">
         <v>26</v>
@@ -1628,7 +1496,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="11" t="s">
         <v>27</v>
@@ -1642,7 +1510,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11" t="s">
         <v>28</v>
@@ -1656,7 +1524,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="11" t="s">
         <v>29</v>
@@ -1715,207 +1583,207 @@
       </c>
       <c r="E52" s="22"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="3"/>
     </row>
-    <row r="61" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D61" s="3"/>
-    </row>
-    <row r="62" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
+    <row r="54" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B62" s="32" t="s">
+      <c r="B54" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C62" s="32"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="16"/>
-      <c r="B63" s="16" t="s">
+      <c r="C54" s="32"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="16"/>
+      <c r="B55" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C63" s="16"/>
-      <c r="D63" s="34">
+      <c r="C55" s="16"/>
+      <c r="D55" s="34">
         <f>E17</f>
         <v>101</v>
       </c>
-      <c r="E63" s="16"/>
+      <c r="E55" s="16"/>
+    </row>
+    <row r="56" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="22"/>
+      <c r="D57" s="36">
+        <v>0</v>
+      </c>
+      <c r="E57" s="22"/>
+      <c r="F57" t="s">
+        <v>72</v>
+      </c>
+      <c r="G57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59" s="25"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="25"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="38"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" s="28"/>
+      <c r="E60" s="11"/>
+      <c r="F60" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="39"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D61" s="40"/>
+      <c r="E61" s="16"/>
+      <c r="F61" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D63" s="41">
+        <f>D55-D64</f>
+        <v>10</v>
+      </c>
+      <c r="E63" s="25"/>
     </row>
     <row r="64" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="3"/>
-    </row>
-    <row r="65" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B65" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C65" s="22"/>
-      <c r="D65" s="36">
-        <v>0</v>
-      </c>
-      <c r="E65" s="22"/>
-      <c r="F65" t="s">
-        <v>72</v>
-      </c>
-      <c r="G65" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="39"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D64" s="19">
+        <v>91</v>
+      </c>
+      <c r="E64" s="16"/>
+      <c r="F64" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C67" s="25"/>
-      <c r="D67" s="26"/>
+      <c r="D67" s="26">
+        <v>7</v>
+      </c>
       <c r="E67" s="25"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="38"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" s="28"/>
+      <c r="F67" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="B68" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="D68" s="28">
+        <v>0</v>
+      </c>
       <c r="E68" s="11"/>
-      <c r="F68" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="39"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D69" s="40"/>
+    </row>
+    <row r="69" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="16"/>
+      <c r="B69" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" s="16"/>
+      <c r="D69" s="42">
+        <f>+D68*100/D67</f>
+        <v>0</v>
+      </c>
       <c r="E69" s="16"/>
-      <c r="F69" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B71" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D71" s="41">
-        <f>D63-D72</f>
-        <v>10</v>
-      </c>
-      <c r="E71" s="25"/>
-    </row>
-    <row r="72" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="39"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D72" s="19">
-        <v>91</v>
-      </c>
-      <c r="E72" s="16"/>
-      <c r="F72" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="D73" s="3"/>
-    </row>
-    <row r="74" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-      <c r="D74" s="3"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B75" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C75" s="25"/>
-      <c r="D75" s="26">
-        <v>7</v>
-      </c>
-      <c r="E75" s="25"/>
-      <c r="F75" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
-      <c r="B76" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C76" s="11"/>
-      <c r="D76" s="28">
-        <v>0</v>
-      </c>
-      <c r="E76" s="11"/>
-    </row>
-    <row r="77" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="16"/>
-      <c r="B77" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C77" s="16"/>
-      <c r="D77" s="42">
-        <f>+D76*100/D75</f>
-        <v>0</v>
-      </c>
-      <c r="E77" s="16"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="50"/>
-      <c r="B80" s="50"/>
-      <c r="D80" s="51"/>
-      <c r="E80" s="51"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="49" t="s">
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="50"/>
+      <c r="B72" s="50"/>
+      <c r="D72" s="51"/>
+      <c r="E72" s="51"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B81" s="49"/>
-      <c r="D81" s="49" t="s">
+      <c r="B73" s="49"/>
+      <c r="D73" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="E81" s="49"/>
+      <c r="E73" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="G7:I12"/>
+    <mergeCell ref="G21:I26"/>
+    <mergeCell ref="G31:H34"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D72:E72"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="85" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="E17" formulaRange="1"/>
   </ignoredErrors>
@@ -1927,13 +1795,12 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>